<commit_message>
FIX simulated data too
</commit_message>
<xml_diff>
--- a/material/simulated_data.xlsx
+++ b/material/simulated_data.xlsx
@@ -386,13 +386,13 @@
         </is>
       </c>
       <c r="B2">
-        <v>3.096009631369112</v>
+        <v>0.747982217853126</v>
       </c>
       <c r="C2">
-        <v>-0.6751288059578144</v>
+        <v>1.272608002624571</v>
       </c>
       <c r="D2">
-        <v>-0.5088415035256617</v>
+        <v>0.3342653064198473</v>
       </c>
     </row>
     <row r="3">
@@ -402,13 +402,13 @@
         </is>
       </c>
       <c r="B3">
-        <v>1.976002031422734</v>
+        <v>2.619778015857148</v>
       </c>
       <c r="C3">
-        <v>1.190300330774065</v>
+        <v>1.924682895761365</v>
       </c>
       <c r="D3">
-        <v>-0.05023823032099994</v>
+        <v>2.376979159805273</v>
       </c>
     </row>
     <row r="4">
@@ -418,13 +418,13 @@
         </is>
       </c>
       <c r="B4">
-        <v>1.558095728720502</v>
+        <v>2.739185677413226</v>
       </c>
       <c r="C4">
-        <v>1.639113527444754</v>
+        <v>-0.4644821689663494</v>
       </c>
       <c r="D4">
-        <v>2.003311980888101</v>
+        <v>-0.6014901743245544</v>
       </c>
     </row>
     <row r="5">
@@ -434,13 +434,13 @@
         </is>
       </c>
       <c r="B5">
-        <v>5.969813594496836</v>
+        <v>6.102051446073806</v>
       </c>
       <c r="C5">
-        <v>0.4125431548890616</v>
+        <v>1.213248978582696</v>
       </c>
       <c r="D5">
-        <v>0.05022157722560205</v>
+        <v>0.4328646475346514</v>
       </c>
     </row>
     <row r="6">
@@ -450,13 +450,13 @@
         </is>
       </c>
       <c r="B6">
-        <v>5.042383743807467</v>
+        <v>4.850344730476794</v>
       </c>
       <c r="C6">
-        <v>1.282323920299547</v>
+        <v>0.05769090177856884</v>
       </c>
       <c r="D6">
-        <v>1.390091249688222</v>
+        <v>0.47118629539715</v>
       </c>
     </row>
     <row r="7">
@@ -466,13 +466,13 @@
         </is>
       </c>
       <c r="B7">
-        <v>4.857695270183349</v>
+        <v>5.440657912325899</v>
       </c>
       <c r="C7">
-        <v>2.150847872550385</v>
+        <v>1.996251390219148</v>
       </c>
       <c r="D7">
-        <v>1.315454926044736</v>
+        <v>1.186194765167633</v>
       </c>
     </row>
   </sheetData>

</xml_diff>